<commit_message>
plot and tabl eupdates
</commit_message>
<xml_diff>
--- a/Output/Classifier Evaluation/Efficiency-Accuracy Table.xlsx
+++ b/Output/Classifier Evaluation/Efficiency-Accuracy Table.xlsx
@@ -537,7 +537,9 @@
           <t>Top 3 Features</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr"/>
+      <c r="C5" s="2" t="n">
+        <v>272.1866018977299</v>
+      </c>
       <c r="D5" s="2" t="n">
         <v>0.06290173530578611</v>
       </c>

</xml_diff>